<commit_message>
HW5 solns; tech report wip
</commit_message>
<xml_diff>
--- a/project/times.xlsx
+++ b/project/times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prholser/ksu/imse884/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2266B1D2-E978-DD4C-ADBF-AF7BDC554A2E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD32DD2D-F8FC-C441-9BE2-AB7BD2AC3408}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{430C9852-43D0-2A4A-9172-0729CD811E64}"/>
+    <workbookView xWindow="1120" yWindow="1220" windowWidth="28040" windowHeight="17440" xr2:uid="{430C9852-43D0-2A4A-9172-0729CD811E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="21">
   <si>
     <t>10_0.2.col</t>
   </si>
@@ -81,10 +81,13 @@
     <t>LR solution times: Assignment formulation, cold restart</t>
   </si>
   <si>
-    <t>LR solution ti+B80</t>
+    <t>LR solution times: Assignment formulation, warm restart</t>
   </si>
   <si>
     <t>LR solution times: Representative formulation, cold restart</t>
+  </si>
+  <si>
+    <t>LR solution times: Representative formulation, warm restart</t>
   </si>
 </sst>
 </file>
@@ -445,21 +448,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D35BC8-0843-6A4C-9B1D-644D9E0CF823}">
-  <dimension ref="A1:X108"/>
+  <dimension ref="A1:X143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D71" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="N93" sqref="N93"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
     <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.1640625" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="24" max="24" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -627,247 +631,234 @@
         <v>6094.6314678199997</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>0.92339801788300002</v>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19">
-        <v>1.4379320144700001</v>
-      </c>
-      <c r="C19">
-        <v>2.6806840896600002</v>
-      </c>
-      <c r="D19">
-        <v>4.5539150238000001</v>
-      </c>
-      <c r="E19">
-        <v>4.54531955719</v>
+        <v>0.92339801788300002</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>1.4219045639000001</v>
+        <v>1.4379320144700001</v>
       </c>
       <c r="C20">
-        <v>3.8656187057500002</v>
+        <v>2.6806840896600002</v>
       </c>
       <c r="D20">
-        <v>5.6054391860999999</v>
+        <v>4.5539150238000001</v>
       </c>
       <c r="E20">
-        <v>5.6113739013700004</v>
+        <v>4.54531955719</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21">
-        <v>1.6724939346300001</v>
+        <v>1.4219045639000001</v>
       </c>
       <c r="C21">
-        <v>2.9726943969700002</v>
+        <v>3.8656187057500002</v>
       </c>
       <c r="D21">
-        <v>8.8299341201800008</v>
+        <v>5.6054391860999999</v>
+      </c>
+      <c r="E21">
+        <v>5.6113739013700004</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>16.0281009674</v>
+        <v>1.6724939346300001</v>
       </c>
       <c r="C22">
-        <v>18.379691124000001</v>
+        <v>2.9726943969700002</v>
       </c>
       <c r="D22">
-        <v>33.579618453999998</v>
+        <v>8.8299341201800008</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>7.78718185425</v>
+        <v>16.0281009674</v>
       </c>
       <c r="C23">
-        <v>72.714415550200002</v>
+        <v>18.379691124000001</v>
       </c>
       <c r="D23">
-        <v>93.612511634800001</v>
+        <v>33.579618453999998</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24">
-        <v>12.4183607101</v>
+        <v>7.78718185425</v>
       </c>
       <c r="C24">
-        <v>147.043985367</v>
+        <v>72.714415550200002</v>
       </c>
       <c r="D24">
-        <v>130.827084541</v>
+        <v>93.612511634800001</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25">
-        <v>13.718767166099999</v>
+        <v>12.4183607101</v>
       </c>
       <c r="C25">
-        <v>133.64249229399999</v>
+        <v>147.043985367</v>
       </c>
       <c r="D25">
-        <v>162.46525764500001</v>
+        <v>130.827084541</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26">
-        <v>178.837831497</v>
+        <v>13.718767166099999</v>
       </c>
       <c r="C26">
-        <v>622.40701198600004</v>
+        <v>133.64249229399999</v>
       </c>
       <c r="D26">
-        <v>183.73250770600001</v>
+        <v>162.46525764500001</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>195.44258594499999</v>
+        <v>178.837831497</v>
       </c>
       <c r="C27">
-        <v>248.67079925499999</v>
+        <v>622.40701198600004</v>
       </c>
       <c r="D27">
-        <v>235.95789814</v>
+        <v>183.73250770600001</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>206.29060649900001</v>
+        <v>195.44258594499999</v>
       </c>
       <c r="C28">
-        <v>304.559673309</v>
+        <v>248.67079925499999</v>
       </c>
       <c r="D28">
-        <v>280.21134853400002</v>
+        <v>235.95789814</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29">
-        <v>116.149162292</v>
+        <v>206.29060649900001</v>
       </c>
       <c r="C29">
-        <v>345.85918808000002</v>
+        <v>304.559673309</v>
       </c>
       <c r="D29">
-        <v>566.69466113999999</v>
+        <v>280.21134853400002</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30">
-        <v>140.86858367900001</v>
+        <v>116.149162292</v>
       </c>
       <c r="C30">
-        <v>1472.0958909999999</v>
+        <v>345.85918808000002</v>
       </c>
       <c r="D30">
-        <v>1235.0087041899999</v>
+        <v>566.69466113999999</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31">
+        <v>140.86858367900001</v>
+      </c>
+      <c r="C31">
+        <v>1472.0958909999999</v>
+      </c>
+      <c r="D31">
+        <v>1235.0087041899999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>149.944394112</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>1889.1868515000001</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>1390.85661602</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34">
-        <v>28</v>
-      </c>
-      <c r="C34">
-        <v>66</v>
-      </c>
-      <c r="D34">
-        <v>67</v>
-      </c>
-      <c r="E34">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35">
         <v>28</v>
       </c>
       <c r="C35">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="D35">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -875,24 +866,27 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C36">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D36">
+        <v>131</v>
+      </c>
+      <c r="E36">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C37">
         <v>120</v>
@@ -903,13 +897,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B38">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="C38">
-        <v>670</v>
+        <v>120</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -917,13 +911,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="C39">
-        <v>1100</v>
+        <v>670</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -931,13 +925,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B40">
-        <v>240</v>
+        <v>110</v>
       </c>
       <c r="C40">
-        <v>2400</v>
+        <v>1100</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -945,13 +939,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41">
-        <v>62</v>
+        <v>240</v>
       </c>
       <c r="C41">
-        <v>930</v>
+        <v>2400</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -959,13 +953,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B42">
-        <v>218</v>
+        <v>62</v>
       </c>
       <c r="C42">
-        <v>3270</v>
+        <v>930</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -973,13 +967,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43">
-        <v>492</v>
+        <v>218</v>
       </c>
       <c r="C43">
-        <v>7380</v>
+        <v>3270</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -987,13 +981,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44">
-        <v>1168</v>
+        <v>492</v>
       </c>
       <c r="C44">
-        <v>17520</v>
+        <v>7380</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1001,13 +995,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B45">
-        <v>248</v>
+        <v>1168</v>
       </c>
       <c r="C45">
-        <v>6198</v>
+        <v>17520</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1015,264 +1009,250 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>248</v>
+      </c>
+      <c r="C46">
+        <v>6198</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>13</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>922</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>23050</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49">
-        <v>0.92339801788300002</v>
+      <c r="D47">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50">
-        <v>1.4379320144700001</v>
-      </c>
-      <c r="C50">
-        <v>1.5179481506300001</v>
-      </c>
-      <c r="D50">
-        <v>0.83842372894299999</v>
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B51">
-        <v>1.4219045639000001</v>
-      </c>
-      <c r="C51">
-        <v>3.1779336929299999</v>
-      </c>
-      <c r="D51">
-        <v>3.0514183044399998</v>
+        <v>0.92339801788300002</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B52">
-        <v>1.6724939346300001</v>
+        <v>1.4379320144700001</v>
       </c>
       <c r="C52">
-        <v>2.4747304916399999</v>
+        <v>1.5179481506300001</v>
       </c>
       <c r="D52">
-        <v>3.7495918273900002</v>
+        <v>0.83842372894299999</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B53">
-        <v>16.0281009674</v>
+        <v>1.4219045639000001</v>
       </c>
       <c r="C53">
-        <v>15.0551795959</v>
+        <v>3.1779336929299999</v>
       </c>
       <c r="D53">
-        <v>20.080204009999999</v>
+        <v>3.0514183044399998</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B54">
-        <v>7.78718185425</v>
+        <v>1.6724939346300001</v>
       </c>
       <c r="C54">
-        <v>55.544541358899998</v>
+        <v>2.4747304916399999</v>
       </c>
       <c r="D54">
-        <v>166.161941528</v>
+        <v>3.7495918273900002</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B55">
-        <v>12.4183607101</v>
+        <v>16.0281009674</v>
       </c>
       <c r="C55">
-        <v>103.78774642899999</v>
+        <v>15.0551795959</v>
       </c>
       <c r="D55">
-        <v>130.712454796</v>
+        <v>20.080204009999999</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B56">
-        <v>13.718767166099999</v>
+        <v>7.78718185425</v>
       </c>
       <c r="C56">
-        <v>101.60833168000001</v>
+        <v>55.544541358899998</v>
       </c>
       <c r="D56">
-        <v>162.062038422</v>
+        <v>166.161941528</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B57">
-        <v>178.837831497</v>
+        <v>12.4183607101</v>
       </c>
       <c r="C57">
-        <v>259.25690841699998</v>
+        <v>103.78774642899999</v>
       </c>
       <c r="D57">
-        <v>220.73734569499999</v>
-      </c>
-      <c r="E57">
-        <v>33.620397567700003</v>
+        <v>130.712454796</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B58">
-        <v>195.44258594499999</v>
+        <v>13.718767166099999</v>
       </c>
       <c r="C58">
-        <v>230.870092392</v>
+        <v>101.60833168000001</v>
       </c>
       <c r="D58">
-        <v>235.88356685599999</v>
+        <v>162.062038422</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B59">
-        <v>206.29060649900001</v>
+        <v>178.837831497</v>
       </c>
       <c r="C59">
-        <v>304.57281780199997</v>
+        <v>259.25690841699998</v>
       </c>
       <c r="D59">
-        <v>279.53382682799997</v>
+        <v>220.73734569499999</v>
+      </c>
+      <c r="E59">
+        <v>33.620397567700003</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B60">
-        <v>116.149162292</v>
+        <v>195.44258594499999</v>
       </c>
       <c r="C60">
-        <v>345.391641617</v>
+        <v>230.870092392</v>
       </c>
       <c r="D60">
-        <v>563.15621376000001</v>
+        <v>235.88356685599999</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B61">
-        <v>140.86858367900001</v>
+        <v>206.29060649900001</v>
       </c>
       <c r="C61">
-        <v>1471.0412550000001</v>
+        <v>304.57281780199997</v>
       </c>
       <c r="D61">
-        <v>1235.2165288900001</v>
+        <v>279.53382682799997</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B62">
-        <v>149.944394112</v>
+        <v>116.149162292</v>
       </c>
       <c r="C62">
-        <v>1887.2403297400001</v>
+        <v>345.391641617</v>
       </c>
       <c r="D62">
-        <v>1389.29991817</v>
+        <v>563.15621376000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63">
+        <v>140.86858367900001</v>
+      </c>
+      <c r="C63">
+        <v>1471.0412550000001</v>
+      </c>
+      <c r="D63">
+        <v>1235.2165288900001</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65">
-        <v>28</v>
-      </c>
-      <c r="C65">
-        <v>41</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
+        <v>149.944394112</v>
+      </c>
+      <c r="C64">
+        <v>1887.2403297400001</v>
+      </c>
+      <c r="D64">
+        <v>1389.29991817</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B66">
-        <v>28</v>
-      </c>
-      <c r="C66">
-        <v>106</v>
-      </c>
-      <c r="D66">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B67">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C67">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -1280,13 +1260,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C68">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -1294,13 +1274,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B69">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="C69">
-        <v>605</v>
+        <v>96</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -1308,13 +1288,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B70">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="C70">
-        <v>990</v>
+        <v>108</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -1322,13 +1302,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B71">
-        <v>240</v>
+        <v>68</v>
       </c>
       <c r="C71">
-        <v>2160</v>
+        <v>605</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -1336,30 +1316,27 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B72">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="C72">
-        <v>845</v>
+        <v>990</v>
       </c>
       <c r="D72">
-        <v>20</v>
-      </c>
-      <c r="E72">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B73">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="C73">
-        <v>3052</v>
+        <v>2160</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -1367,27 +1344,30 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B74">
-        <v>492</v>
+        <v>62</v>
       </c>
       <c r="C74">
-        <v>6888</v>
+        <v>845</v>
       </c>
       <c r="D74">
+        <v>20</v>
+      </c>
+      <c r="E74">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B75">
-        <v>1168</v>
+        <v>218</v>
       </c>
       <c r="C75">
-        <v>16352</v>
+        <v>3052</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -1395,13 +1375,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B76">
-        <v>248</v>
+        <v>492</v>
       </c>
       <c r="C76">
-        <v>5950</v>
+        <v>6888</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -1409,398 +1389,1156 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B77">
-        <v>922</v>
+        <v>1168</v>
       </c>
       <c r="C77">
-        <v>22128</v>
+        <v>16352</v>
       </c>
       <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78">
+        <v>248</v>
+      </c>
+      <c r="C78">
+        <v>5950</v>
+      </c>
+      <c r="D78">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>16</v>
-      </c>
-      <c r="B79" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>0</v>
-      </c>
-      <c r="B80">
-        <v>0.114322662354</v>
-      </c>
-    </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>1</v>
-      </c>
-      <c r="B81">
-        <v>0.15234661102300001</v>
-      </c>
-      <c r="C81">
-        <v>0.14074420929000001</v>
+        <v>13</v>
+      </c>
+      <c r="B79">
+        <v>922</v>
+      </c>
+      <c r="C79">
+        <v>22128</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>2</v>
-      </c>
-      <c r="B82">
-        <v>0.13333702087400001</v>
-      </c>
-      <c r="C82">
-        <v>0.14618015289299999</v>
+        <v>16</v>
+      </c>
+      <c r="B82" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B83">
-        <v>8.3336830139199999E-2</v>
-      </c>
-      <c r="C83">
-        <v>8.0457687377900003E-2</v>
+        <v>0.114322662354</v>
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B84">
-        <v>5.0531435012800001</v>
+        <v>0.15234661102300001</v>
       </c>
       <c r="C84">
-        <v>5.7965383529699999</v>
-      </c>
-      <c r="D84">
-        <v>6.4531517028799996</v>
-      </c>
-      <c r="E84">
-        <v>4.64278888702</v>
-      </c>
-      <c r="F84">
-        <v>4.3826608657800001</v>
+        <v>0.14074420929000001</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B85">
-        <v>6.4734373092700004</v>
+        <v>0.13333702087400001</v>
       </c>
       <c r="C85">
-        <v>9.53453540802</v>
-      </c>
-      <c r="D85">
-        <v>10.262032508900001</v>
+        <v>0.14618015289299999</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B86">
-        <v>4.7660646438600001</v>
+        <v>8.3336830139199999E-2</v>
       </c>
       <c r="C86">
-        <v>4.40786552429</v>
-      </c>
-      <c r="D86">
-        <v>5.3999528884899997</v>
-      </c>
-      <c r="E86">
-        <v>3.8970851898199999</v>
+        <v>8.0457687377900003E-2</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B87">
-        <v>0.19862747192399999</v>
+        <v>5.0531435012800001</v>
       </c>
       <c r="C87">
-        <v>0.18180942535399999</v>
+        <v>5.7965383529699999</v>
+      </c>
+      <c r="D87">
+        <v>6.4531517028799996</v>
+      </c>
+      <c r="E87">
+        <v>4.64278888702</v>
+      </c>
+      <c r="F87">
+        <v>4.3826608657800001</v>
       </c>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B88">
-        <v>155.828081131</v>
+        <v>6.4734373092700004</v>
       </c>
       <c r="C88">
-        <v>127.199456215</v>
+        <v>9.53453540802</v>
       </c>
       <c r="D88">
-        <v>157.192998886</v>
-      </c>
-      <c r="E88">
-        <v>178.771111488</v>
-      </c>
-      <c r="F88">
-        <v>115.276694298</v>
+        <v>10.262032508900001</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B89">
-        <v>132.576334</v>
+        <v>4.7660646438600001</v>
       </c>
       <c r="C89">
-        <v>172.72638606999999</v>
+        <v>4.40786552429</v>
       </c>
       <c r="D89">
-        <v>243.84692668899999</v>
+        <v>5.3999528884899997</v>
       </c>
       <c r="E89">
-        <v>300.869763374</v>
-      </c>
-      <c r="F89">
-        <v>271.63347911800003</v>
+        <v>3.8970851898199999</v>
       </c>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B90">
-        <v>60.065791130100003</v>
+        <v>0.19862747192399999</v>
       </c>
       <c r="C90">
-        <v>62.084241867099998</v>
-      </c>
-      <c r="D90">
-        <v>81.618421554600005</v>
-      </c>
-      <c r="E90">
-        <v>107.59427166</v>
-      </c>
-      <c r="F90">
-        <v>100.069432259</v>
-      </c>
-      <c r="G90">
-        <v>88.865528106699998</v>
+        <v>0.18180942535399999</v>
       </c>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B91">
-        <v>6.5477800369299999</v>
+        <v>155.828081131</v>
       </c>
       <c r="C91">
-        <v>11.421333313</v>
+        <v>127.199456215</v>
       </c>
       <c r="D91">
-        <v>11.9752645493</v>
+        <v>157.192998886</v>
       </c>
       <c r="E91">
-        <v>12.143657684300001</v>
+        <v>178.771111488</v>
       </c>
       <c r="F91">
-        <v>14.2650222778</v>
+        <v>115.276694298</v>
       </c>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B92">
-        <v>274.264140129</v>
+        <v>132.576334</v>
       </c>
       <c r="C92">
-        <v>918.77144146000001</v>
+        <v>172.72638606999999</v>
       </c>
       <c r="D92">
-        <v>803.14160346999995</v>
+        <v>243.84692668899999</v>
       </c>
       <c r="E92">
-        <v>802.39203071600002</v>
+        <v>300.869763374</v>
       </c>
       <c r="F92">
-        <v>834.89426135999997</v>
-      </c>
-      <c r="G92">
-        <v>814.30641841900001</v>
-      </c>
-      <c r="H92">
-        <v>841.62020397200001</v>
-      </c>
-      <c r="I92">
-        <v>814.43115138999997</v>
-      </c>
-      <c r="J92">
-        <v>810.49060344700001</v>
-      </c>
-      <c r="K92">
-        <v>841.41893482199998</v>
-      </c>
-      <c r="L92">
-        <v>815.26906585699999</v>
-      </c>
-      <c r="M92">
-        <v>846.94985675800001</v>
-      </c>
-      <c r="N92">
-        <v>846.84141922000003</v>
-      </c>
-      <c r="O92">
-        <v>818.34191799200005</v>
-      </c>
-      <c r="P92">
-        <v>819.49999523199995</v>
-      </c>
-      <c r="Q92">
-        <v>845.86744880699996</v>
-      </c>
-      <c r="R92">
-        <v>812.04125785799999</v>
-      </c>
-      <c r="S92">
-        <v>837.59671497299996</v>
-      </c>
-      <c r="T92">
-        <v>836.48554229700005</v>
-      </c>
-      <c r="U92">
-        <v>845.83357334100003</v>
-      </c>
-      <c r="V92">
-        <v>816.05400085400004</v>
-      </c>
-      <c r="W92">
-        <v>874.78560066199998</v>
-      </c>
-      <c r="X92">
-        <v>846.91305065200004</v>
+        <v>271.63347911800003</v>
       </c>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B93">
-        <v>696.04763031000005</v>
+        <v>60.065791130100003</v>
       </c>
       <c r="C93">
-        <v>825.82221221899999</v>
+        <v>62.084241867099998</v>
       </c>
       <c r="D93">
-        <v>839.31715774500003</v>
+        <v>81.618421554600005</v>
       </c>
       <c r="E93">
-        <v>935.72770690899995</v>
+        <v>107.59427166</v>
       </c>
       <c r="F93">
-        <v>968.06043052699999</v>
+        <v>100.069432259</v>
       </c>
       <c r="G93">
-        <v>1106.9918899500001</v>
-      </c>
-      <c r="H93">
-        <v>1013.51549721</v>
-      </c>
-      <c r="I93">
-        <v>1008.3247585300001</v>
-      </c>
-      <c r="J93">
-        <v>1075.22230816</v>
-      </c>
-      <c r="K93">
-        <v>1101.0358180999999</v>
-      </c>
-      <c r="L93">
-        <v>1095.9455280300001</v>
-      </c>
-      <c r="M93">
-        <v>1032.83968258</v>
+        <v>88.865528106699998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>11</v>
+      </c>
+      <c r="B94">
+        <v>6.5477800369299999</v>
+      </c>
+      <c r="C94">
+        <v>11.421333313</v>
+      </c>
+      <c r="D94">
+        <v>11.9752645493</v>
+      </c>
+      <c r="E94">
+        <v>12.143657684300001</v>
+      </c>
+      <c r="F94">
+        <v>14.2650222778</v>
       </c>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>274.264140129</v>
+      </c>
+      <c r="C95">
+        <v>918.77144146000001</v>
+      </c>
+      <c r="D95">
+        <v>803.14160346999995</v>
+      </c>
+      <c r="E95">
+        <v>802.39203071600002</v>
+      </c>
+      <c r="F95">
+        <v>834.89426135999997</v>
+      </c>
+      <c r="G95">
+        <v>814.30641841900001</v>
+      </c>
+      <c r="H95">
+        <v>841.62020397200001</v>
+      </c>
+      <c r="I95">
+        <v>814.43115138999997</v>
+      </c>
+      <c r="J95">
+        <v>810.49060344700001</v>
+      </c>
+      <c r="K95">
+        <v>841.41893482199998</v>
+      </c>
+      <c r="L95">
+        <v>815.26906585699999</v>
+      </c>
+      <c r="M95">
+        <v>846.94985675800001</v>
+      </c>
+      <c r="N95">
+        <v>846.84141922000003</v>
+      </c>
+      <c r="O95">
+        <v>818.34191799200005</v>
+      </c>
+      <c r="P95">
+        <v>819.49999523199995</v>
+      </c>
+      <c r="Q95">
+        <v>845.86744880699996</v>
+      </c>
+      <c r="R95">
+        <v>812.04125785799999</v>
+      </c>
+      <c r="S95">
+        <v>837.59671497299996</v>
+      </c>
+      <c r="T95">
+        <v>836.48554229700005</v>
+      </c>
+      <c r="U95">
+        <v>845.83357334100003</v>
+      </c>
+      <c r="V95">
+        <v>816.05400085400004</v>
+      </c>
+      <c r="W95">
+        <v>874.78560066199998</v>
+      </c>
+      <c r="X95">
+        <v>846.91305065200004</v>
       </c>
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>13</v>
+      </c>
+      <c r="B96">
+        <v>696.04763031000005</v>
+      </c>
+      <c r="C96">
+        <v>825.82221221899999</v>
+      </c>
+      <c r="D96">
+        <v>839.31715774500003</v>
+      </c>
+      <c r="E96">
+        <v>935.72770690899995</v>
+      </c>
+      <c r="F96">
+        <v>968.06043052699999</v>
+      </c>
+      <c r="G96">
+        <v>1106.9918899500001</v>
+      </c>
+      <c r="H96">
+        <v>1013.51549721</v>
+      </c>
+      <c r="I96">
+        <v>1008.3247585300001</v>
+      </c>
+      <c r="J96">
+        <v>1075.22230816</v>
+      </c>
+      <c r="K96">
+        <v>1101.0358180999999</v>
+      </c>
+      <c r="L96">
+        <v>1095.9455280300001</v>
+      </c>
+      <c r="M96">
+        <v>1032.83968258</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="B99">
+        <v>6</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="B100">
+        <v>5</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="B102">
+        <v>20</v>
+      </c>
+      <c r="C102">
+        <v>38</v>
+      </c>
+      <c r="D102">
+        <v>39</v>
+      </c>
+      <c r="E102">
+        <v>40</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="B103">
+        <v>75</v>
+      </c>
+      <c r="C103">
+        <v>107</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="B104">
+        <v>60</v>
+      </c>
+      <c r="C104">
+        <v>76</v>
+      </c>
+      <c r="D104">
+        <v>78</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="B106">
+        <v>220</v>
+      </c>
+      <c r="C106">
+        <v>339</v>
+      </c>
+      <c r="D106">
+        <v>374</v>
+      </c>
+      <c r="E106">
+        <v>386</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="B107">
+        <v>589</v>
+      </c>
+      <c r="C107">
+        <v>827</v>
+      </c>
+      <c r="D107">
+        <v>835</v>
+      </c>
+      <c r="E107">
+        <v>836</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="B108">
+        <v>340</v>
+      </c>
+      <c r="C108">
+        <v>429</v>
+      </c>
+      <c r="D108">
+        <v>478</v>
+      </c>
+      <c r="E108">
+        <v>487</v>
+      </c>
+      <c r="F108">
+        <v>495</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="B109">
+        <v>50</v>
+      </c>
+      <c r="C109">
+        <v>67</v>
+      </c>
+      <c r="D109">
+        <v>80</v>
+      </c>
+      <c r="E109">
+        <v>91</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="B110">
+        <v>1848</v>
+      </c>
+      <c r="C110">
+        <v>2706</v>
+      </c>
+      <c r="D110">
+        <v>2897</v>
+      </c>
+      <c r="E110">
+        <v>2960</v>
+      </c>
+      <c r="F110">
+        <v>2969</v>
+      </c>
+      <c r="G110">
+        <v>2989</v>
+      </c>
+      <c r="H110">
+        <v>2994</v>
+      </c>
+      <c r="I110">
+        <v>3003</v>
+      </c>
+      <c r="J110">
+        <v>3006</v>
+      </c>
+      <c r="K110">
+        <v>3011</v>
+      </c>
+      <c r="L110">
+        <v>3015</v>
+      </c>
+      <c r="M110">
+        <v>3023</v>
+      </c>
+      <c r="N110">
+        <v>3027</v>
+      </c>
+      <c r="O110">
+        <v>3028</v>
+      </c>
+      <c r="P110">
+        <v>3030</v>
+      </c>
+      <c r="Q110">
+        <v>3032</v>
+      </c>
+      <c r="R110">
+        <v>3033</v>
+      </c>
+      <c r="S110">
+        <v>3034</v>
+      </c>
+      <c r="T110">
+        <v>3036</v>
+      </c>
+      <c r="U110">
+        <v>3037</v>
+      </c>
+      <c r="V110">
+        <v>3038</v>
+      </c>
+      <c r="W110">
+        <v>3039</v>
+      </c>
+      <c r="X110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>13</v>
+      </c>
+      <c r="B111">
+        <v>3308</v>
+      </c>
+      <c r="C111">
+        <v>4456</v>
+      </c>
+      <c r="D111">
+        <v>4886</v>
+      </c>
+      <c r="E111">
+        <v>5007</v>
+      </c>
+      <c r="F111">
+        <v>5083</v>
+      </c>
+      <c r="G111">
+        <v>5089</v>
+      </c>
+      <c r="H111">
+        <v>5095</v>
+      </c>
+      <c r="I111">
+        <v>5100</v>
+      </c>
+      <c r="J111">
+        <v>5102</v>
+      </c>
+      <c r="K111">
+        <v>5015</v>
+      </c>
+      <c r="L111">
+        <v>5016</v>
+      </c>
+      <c r="M111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115">
+        <v>0.114322662354</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>1</v>
+      </c>
+      <c r="B116">
+        <v>0.15234661102300001</v>
+      </c>
+      <c r="C116">
+        <v>6.6526412963899995E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117">
+        <v>0.13333702087400001</v>
+      </c>
+      <c r="C117">
+        <v>4.4780731201199998E-2</v>
+      </c>
+      <c r="D117">
+        <v>4.59699630737E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118">
+        <v>8.3336830139199999E-2</v>
+      </c>
+      <c r="C118">
+        <v>2.7288436889600001E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119">
+        <v>5.0531435012800001</v>
+      </c>
+      <c r="C119">
+        <v>1.8691864013699999</v>
+      </c>
+      <c r="D119">
+        <v>1.5256567001300001</v>
+      </c>
+      <c r="E119">
+        <v>1.7287378311199999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120">
+        <v>6.4734373092700004</v>
+      </c>
+      <c r="C120">
+        <v>3.6447629928600001</v>
+      </c>
+      <c r="D120">
+        <v>3.3896007537799999</v>
+      </c>
+      <c r="E120">
+        <v>0.52612972259500002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121">
+        <v>4.7660646438600001</v>
+      </c>
+      <c r="C121">
+        <v>3.0248231887800001</v>
+      </c>
+      <c r="D121">
+        <v>2.50283336639</v>
+      </c>
+      <c r="E121">
+        <v>0.296401023865</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122">
+        <v>0.19862747192399999</v>
+      </c>
+      <c r="C122">
+        <v>6.3437461853000005E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>8</v>
+      </c>
+      <c r="B123">
+        <v>155.828081131</v>
+      </c>
+      <c r="C123">
+        <v>65.464577674899999</v>
+      </c>
+      <c r="D123">
+        <v>59.817117691</v>
+      </c>
+      <c r="E123">
+        <v>28.5555524826</v>
+      </c>
+      <c r="F123">
+        <v>23.190909385699999</v>
+      </c>
+      <c r="G123">
+        <v>5.1553182601899996</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124">
+        <v>132.576334</v>
+      </c>
+      <c r="C124">
+        <v>88.898946762099996</v>
+      </c>
+      <c r="D124">
+        <v>139.406115532</v>
+      </c>
+      <c r="E124">
+        <v>64.340105056799999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>10</v>
+      </c>
+      <c r="B125">
+        <v>60.065791130100003</v>
+      </c>
+      <c r="C125">
+        <v>36.169199943499997</v>
+      </c>
+      <c r="D125">
+        <v>48.572656631500003</v>
+      </c>
+      <c r="E125">
+        <v>32.4627075195</v>
+      </c>
+      <c r="F125">
+        <v>7.5039157867400004</v>
+      </c>
+      <c r="G125">
+        <v>2.48493289948</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>11</v>
+      </c>
+      <c r="B126">
+        <v>6.5477800369299999</v>
+      </c>
+      <c r="C126">
+        <v>10.210365295400001</v>
+      </c>
+      <c r="D126">
+        <v>4.5209894180300001</v>
+      </c>
+      <c r="E126">
+        <v>1.5552186965899999</v>
+      </c>
+      <c r="F126">
+        <v>1.38092708588</v>
+      </c>
+      <c r="G126">
+        <v>1.1399354934699999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>12</v>
+      </c>
+      <c r="B127">
+        <v>274.264140129</v>
+      </c>
+      <c r="C127">
+        <v>914.25992107399998</v>
+      </c>
+      <c r="D127">
+        <v>796.42307758300001</v>
+      </c>
+      <c r="E127">
+        <v>795.99016952500006</v>
+      </c>
+      <c r="F127">
+        <v>798.30110073100002</v>
+      </c>
+      <c r="G127">
+        <v>204.56955146799999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>13</v>
+      </c>
+      <c r="B128">
+        <v>696.04651737200004</v>
+      </c>
+      <c r="C128">
+        <v>825.04453468300005</v>
+      </c>
+      <c r="D128">
+        <v>837.79569625900001</v>
+      </c>
+      <c r="E128">
+        <v>934.11157798800002</v>
+      </c>
+      <c r="F128">
+        <v>967.52824211100005</v>
+      </c>
+      <c r="G128">
+        <v>553.90704345699999</v>
+      </c>
+      <c r="H128">
+        <v>291.21484184299999</v>
+      </c>
+      <c r="I128">
+        <v>73.556304931599996</v>
+      </c>
+      <c r="J128">
+        <v>23.8482675552</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>6</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132">
+        <v>5</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>3</v>
+      </c>
+      <c r="B133">
+        <v>2</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>4</v>
+      </c>
+      <c r="B134">
+        <v>20</v>
+      </c>
+      <c r="C134">
+        <v>10</v>
+      </c>
+      <c r="D134">
+        <v>5</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>5</v>
+      </c>
+      <c r="B135">
+        <v>75</v>
+      </c>
+      <c r="C135">
+        <v>24</v>
+      </c>
+      <c r="D135">
+        <v>8</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>6</v>
+      </c>
+      <c r="B136">
+        <v>60</v>
+      </c>
+      <c r="C136">
+        <v>20</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>7</v>
+      </c>
+      <c r="B137">
+        <v>4</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B138">
+        <v>220</v>
+      </c>
+      <c r="C138">
+        <v>129</v>
+      </c>
+      <c r="D138">
+        <v>42</v>
+      </c>
+      <c r="E138">
+        <v>7</v>
+      </c>
+      <c r="F138">
+        <v>2</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>9</v>
+      </c>
+      <c r="B139">
+        <v>589</v>
+      </c>
+      <c r="C139">
+        <v>246</v>
+      </c>
+      <c r="D139">
+        <v>9</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>10</v>
+      </c>
+      <c r="B140">
+        <v>340</v>
+      </c>
+      <c r="C140">
+        <v>102</v>
+      </c>
+      <c r="D140">
+        <v>57</v>
+      </c>
+      <c r="E140">
+        <v>4</v>
+      </c>
+      <c r="F140">
+        <v>4</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>11</v>
+      </c>
+      <c r="B141">
+        <v>50</v>
+      </c>
+      <c r="C141">
+        <v>19</v>
+      </c>
+      <c r="D141">
+        <v>8</v>
+      </c>
+      <c r="E141">
+        <v>2</v>
+      </c>
+      <c r="F141">
+        <v>3</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>12</v>
+      </c>
+      <c r="B142">
+        <v>1848</v>
+      </c>
+      <c r="C142">
+        <v>858</v>
+      </c>
+      <c r="D142">
+        <v>191</v>
+      </c>
+      <c r="E142">
+        <v>63</v>
+      </c>
+      <c r="F142">
+        <v>4</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>13</v>
+      </c>
+      <c r="B143">
+        <v>3308</v>
+      </c>
+      <c r="C143">
+        <v>1148</v>
+      </c>
+      <c r="D143">
+        <v>430</v>
+      </c>
+      <c r="E143">
+        <v>121</v>
+      </c>
+      <c r="F143">
+        <v>76</v>
+      </c>
+      <c r="G143">
+        <v>9</v>
+      </c>
+      <c r="H143">
+        <v>5</v>
+      </c>
+      <c r="I143">
+        <v>5</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>